<commit_message>
plan updated by Leo March 4,2015
</commit_message>
<xml_diff>
--- a/management/MLMplan.xlsx
+++ b/management/MLMplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="0" windowWidth="21840" windowHeight="13740" activeTab="4"/>
+    <workbookView xWindow="735" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="文件封面" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0">
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
   <si>
     <t>密级：</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -447,15 +447,6 @@
     <t>signin.bmml</t>
   </si>
   <si>
-    <t>registration2.bmml</t>
-  </si>
-  <si>
-    <t>registration1-1.bmml</t>
-  </si>
-  <si>
-    <t>registration1.bmml</t>
-  </si>
-  <si>
     <t>products.bmml</t>
   </si>
   <si>
@@ -547,6 +538,27 @@
   </si>
   <si>
     <t>需要与需求方确认一下UI设计有无问题</t>
+  </si>
+  <si>
+    <t>selectaccount.bmml</t>
+  </si>
+  <si>
+    <t>selectautoship.bmml</t>
+  </si>
+  <si>
+    <t>registration.bmml</t>
+  </si>
+  <si>
+    <t>productmaintenance.bmml</t>
+  </si>
+  <si>
+    <t>currencymaintenance.bmml</t>
+  </si>
+  <si>
+    <t>countrymaintenance.bmml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All UI static pages coding for front end </t>
   </si>
 </sst>
 </file>
@@ -554,10 +566,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="165" formatCode="0.0\ &quot;人月&quot;"/>
-    <numFmt numFmtId="166" formatCode="0\ &quot;天&quot;\ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="166" formatCode="0.0\ &quot;人月&quot;"/>
+    <numFmt numFmtId="167" formatCode="0\ &quot;天&quot;\ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -2008,7 +2020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
@@ -2168,7 +2180,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -2196,7 +2208,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -2212,7 +2224,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -2224,7 +2236,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -2256,7 +2268,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -2284,7 +2296,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -2494,10 +2506,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="20" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2966,6 +2978,22 @@
     <xf numFmtId="0" fontId="33" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="34" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3008,6 +3036,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="69" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3072,17 +3112,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="69" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="70" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3096,29 +3142,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="34" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3133,23 +3162,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3160,15 +3172,257 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规_B-Box system project weekreport0525" xfId="5"/>
     <cellStyle name="常规_sst121" xfId="3"/>
     <cellStyle name="常规_sst3C" xfId="2"/>
     <cellStyle name="常规_风险管理计划模板" xfId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="1" builtinId="6"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3331,83 +3585,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9900FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3657,7 +3834,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4545,32 +4722,32 @@
       <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A3" s="271" t="s">
+      <c r="A3" s="276" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="271"/>
-      <c r="C3" s="271"/>
-      <c r="D3" s="271"/>
-      <c r="E3" s="271"/>
-      <c r="F3" s="271"/>
-      <c r="G3" s="271"/>
+      <c r="B3" s="276"/>
+      <c r="C3" s="276"/>
+      <c r="D3" s="276"/>
+      <c r="E3" s="276"/>
+      <c r="F3" s="276"/>
+      <c r="G3" s="276"/>
       <c r="H3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="271" t="s">
+      <c r="A4" s="276" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="271"/>
-      <c r="C4" s="271"/>
-      <c r="D4" s="271"/>
-      <c r="E4" s="271"/>
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="272" t="s">
+      <c r="G4" s="277" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="272"/>
+      <c r="H4" s="277"/>
     </row>
     <row r="5" spans="1:8" ht="22.5">
       <c r="A5" s="10"/>
@@ -4623,25 +4800,25 @@
       <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="276" t="s">
+      <c r="D10" s="281" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="277"/>
-      <c r="F10" s="277"/>
+      <c r="E10" s="282"/>
+      <c r="F10" s="282"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="46.5" customHeight="1">
-      <c r="A11" s="273" t="s">
+      <c r="A11" s="278" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="273"/>
-      <c r="C11" s="273"/>
-      <c r="D11" s="273"/>
-      <c r="E11" s="273"/>
-      <c r="F11" s="273"/>
-      <c r="G11" s="273"/>
-      <c r="H11" s="273"/>
+      <c r="B11" s="278"/>
+      <c r="C11" s="278"/>
+      <c r="D11" s="278"/>
+      <c r="E11" s="278"/>
+      <c r="F11" s="278"/>
+      <c r="G11" s="278"/>
+      <c r="H11" s="278"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="15.75">
       <c r="A12" s="12"/>
@@ -4678,23 +4855,23 @@
       <c r="A16" s="12"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="275" t="s">
+      <c r="D16" s="280" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="275"/>
-      <c r="F16" s="275"/>
+      <c r="E16" s="280"/>
+      <c r="F16" s="280"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="22.5">
-      <c r="A17" s="274"/>
-      <c r="B17" s="274"/>
-      <c r="C17" s="274"/>
-      <c r="D17" s="274"/>
-      <c r="E17" s="274"/>
-      <c r="F17" s="274"/>
-      <c r="G17" s="274"/>
-      <c r="H17" s="274"/>
+      <c r="A17" s="279"/>
+      <c r="B17" s="279"/>
+      <c r="C17" s="279"/>
+      <c r="D17" s="279"/>
+      <c r="E17" s="279"/>
+      <c r="F17" s="279"/>
+      <c r="G17" s="279"/>
+      <c r="H17" s="279"/>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1" ht="15.75">
       <c r="A18" s="12"/>
@@ -4807,16 +4984,16 @@
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A29" s="268" t="s">
+      <c r="A29" s="273" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="269"/>
-      <c r="C29" s="269"/>
-      <c r="D29" s="269"/>
-      <c r="E29" s="269"/>
-      <c r="F29" s="269"/>
-      <c r="G29" s="269"/>
-      <c r="H29" s="269"/>
+      <c r="B29" s="274"/>
+      <c r="C29" s="274"/>
+      <c r="D29" s="274"/>
+      <c r="E29" s="274"/>
+      <c r="F29" s="274"/>
+      <c r="G29" s="274"/>
+      <c r="H29" s="274"/>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="15.75">
       <c r="A30" s="12"/>
@@ -4876,15 +5053,15 @@
       <c r="A34" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="270"/>
-      <c r="C34" s="270"/>
-      <c r="D34" s="270"/>
+      <c r="B34" s="275"/>
+      <c r="C34" s="275"/>
+      <c r="D34" s="275"/>
       <c r="E34" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="270"/>
-      <c r="G34" s="270"/>
-      <c r="H34" s="270"/>
+      <c r="F34" s="275"/>
+      <c r="G34" s="275"/>
+      <c r="H34" s="275"/>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" ht="15.75">
       <c r="A35" s="12" t="s">
@@ -5281,8 +5458,8 @@
         <v>1</v>
       </c>
       <c r="D4" s="79"/>
-      <c r="E4" s="280"/>
-      <c r="F4" s="281"/>
+      <c r="E4" s="285"/>
+      <c r="F4" s="286"/>
       <c r="G4" s="96"/>
     </row>
     <row r="5" spans="1:8">
@@ -5291,8 +5468,8 @@
         <v>2</v>
       </c>
       <c r="D5" s="79"/>
-      <c r="E5" s="280"/>
-      <c r="F5" s="281"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="286"/>
       <c r="G5" s="96"/>
     </row>
     <row r="6" spans="1:8">
@@ -5301,8 +5478,8 @@
         <v>3</v>
       </c>
       <c r="D6" s="79"/>
-      <c r="E6" s="280"/>
-      <c r="F6" s="281"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="286"/>
       <c r="G6" s="96"/>
     </row>
     <row r="7" spans="1:8">
@@ -5311,8 +5488,8 @@
         <v>4</v>
       </c>
       <c r="D7" s="79"/>
-      <c r="E7" s="280"/>
-      <c r="F7" s="281"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="286"/>
       <c r="G7" s="96"/>
     </row>
     <row r="8" spans="1:8">
@@ -5321,8 +5498,8 @@
         <v>5</v>
       </c>
       <c r="D8" s="79"/>
-      <c r="E8" s="280"/>
-      <c r="F8" s="281"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="286"/>
       <c r="G8" s="96"/>
     </row>
     <row r="9" spans="1:8">
@@ -5331,8 +5508,8 @@
         <v>6</v>
       </c>
       <c r="D9" s="79"/>
-      <c r="E9" s="280"/>
-      <c r="F9" s="281"/>
+      <c r="E9" s="285"/>
+      <c r="F9" s="286"/>
       <c r="G9" s="96"/>
     </row>
     <row r="10" spans="1:8">
@@ -5341,24 +5518,24 @@
         <v>7</v>
       </c>
       <c r="D10" s="79"/>
-      <c r="E10" s="280"/>
-      <c r="F10" s="281"/>
+      <c r="E10" s="285"/>
+      <c r="F10" s="286"/>
       <c r="G10" s="96"/>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" s="94"/>
       <c r="C11" s="81"/>
       <c r="D11" s="79"/>
-      <c r="E11" s="280"/>
-      <c r="F11" s="281"/>
+      <c r="E11" s="285"/>
+      <c r="F11" s="286"/>
       <c r="G11" s="96"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1">
       <c r="B12" s="97"/>
       <c r="C12" s="98"/>
       <c r="D12" s="99"/>
-      <c r="E12" s="278"/>
-      <c r="F12" s="279"/>
+      <c r="E12" s="283"/>
+      <c r="F12" s="284"/>
       <c r="G12" s="100"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1">
@@ -6707,7 +6884,7 @@
       <c r="A4" s="120"/>
       <c r="B4" s="121"/>
       <c r="C4" s="122"/>
-      <c r="D4" s="290" t="s">
+      <c r="D4" s="298" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="249"/>
@@ -6717,14 +6894,14 @@
       <c r="G4" s="124"/>
       <c r="H4" s="125"/>
       <c r="I4" s="126"/>
-      <c r="J4" s="292" t="s">
+      <c r="J4" s="300" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="127" customFormat="1" ht="17.45" customHeight="1">
       <c r="B5" s="128"/>
       <c r="C5" s="129"/>
-      <c r="D5" s="291"/>
+      <c r="D5" s="299"/>
       <c r="E5" s="208" t="s">
         <v>58</v>
       </c>
@@ -6740,17 +6917,17 @@
       <c r="I5" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="293"/>
+      <c r="J5" s="301"/>
     </row>
     <row r="6" spans="1:11" s="127" customFormat="1" ht="16.5" customHeight="1">
       <c r="A6" s="120"/>
       <c r="B6" s="121"/>
       <c r="C6" s="132"/>
       <c r="D6" s="133" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E6" s="250" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F6" s="134"/>
       <c r="G6" s="135"/>
@@ -6763,10 +6940,10 @@
       <c r="B7" s="121"/>
       <c r="C7" s="132"/>
       <c r="D7" s="133" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="250" t="s">
         <v>92</v>
-      </c>
-      <c r="E7" s="250" t="s">
-        <v>95</v>
       </c>
       <c r="F7" s="134"/>
       <c r="G7" s="135"/>
@@ -6779,10 +6956,10 @@
       <c r="B8" s="121"/>
       <c r="C8" s="132"/>
       <c r="D8" s="133" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E8" s="250" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F8" s="134"/>
       <c r="G8" s="135"/>
@@ -7080,158 +7257,158 @@
       <c r="D28" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="297" t="s">
+      <c r="E28" s="305" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="298"/>
-      <c r="G28" s="294" t="s">
+      <c r="F28" s="306"/>
+      <c r="G28" s="302" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="295"/>
-      <c r="I28" s="296"/>
+      <c r="H28" s="303"/>
+      <c r="I28" s="304"/>
     </row>
     <row r="29" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A29" s="120"/>
       <c r="B29" s="121"/>
       <c r="C29" s="132"/>
       <c r="D29" s="133"/>
-      <c r="E29" s="288"/>
-      <c r="F29" s="289"/>
-      <c r="G29" s="282"/>
-      <c r="H29" s="283"/>
-      <c r="I29" s="284"/>
+      <c r="E29" s="296"/>
+      <c r="F29" s="297"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="291"/>
+      <c r="I29" s="292"/>
     </row>
     <row r="30" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A30" s="120"/>
       <c r="B30" s="121"/>
       <c r="C30" s="132"/>
       <c r="D30" s="133"/>
-      <c r="E30" s="288"/>
-      <c r="F30" s="289"/>
-      <c r="G30" s="282"/>
-      <c r="H30" s="283"/>
-      <c r="I30" s="284"/>
+      <c r="E30" s="296"/>
+      <c r="F30" s="297"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="291"/>
+      <c r="I30" s="292"/>
     </row>
     <row r="31" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A31" s="120"/>
       <c r="B31" s="121"/>
       <c r="C31" s="132"/>
       <c r="D31" s="133"/>
-      <c r="E31" s="288"/>
-      <c r="F31" s="289"/>
-      <c r="G31" s="285"/>
-      <c r="H31" s="286"/>
-      <c r="I31" s="287"/>
+      <c r="E31" s="296"/>
+      <c r="F31" s="297"/>
+      <c r="G31" s="293"/>
+      <c r="H31" s="294"/>
+      <c r="I31" s="295"/>
     </row>
     <row r="32" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A32" s="120"/>
       <c r="B32" s="121"/>
       <c r="C32" s="132"/>
       <c r="D32" s="133"/>
-      <c r="E32" s="288"/>
-      <c r="F32" s="289"/>
-      <c r="G32" s="285"/>
-      <c r="H32" s="286"/>
-      <c r="I32" s="287"/>
+      <c r="E32" s="296"/>
+      <c r="F32" s="297"/>
+      <c r="G32" s="293"/>
+      <c r="H32" s="294"/>
+      <c r="I32" s="295"/>
     </row>
     <row r="33" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A33" s="120"/>
       <c r="B33" s="121"/>
       <c r="C33" s="132"/>
       <c r="D33" s="133"/>
-      <c r="E33" s="288"/>
-      <c r="F33" s="289"/>
-      <c r="G33" s="285"/>
-      <c r="H33" s="286"/>
-      <c r="I33" s="287"/>
+      <c r="E33" s="296"/>
+      <c r="F33" s="297"/>
+      <c r="G33" s="293"/>
+      <c r="H33" s="294"/>
+      <c r="I33" s="295"/>
     </row>
     <row r="34" spans="1:10" s="127" customFormat="1" ht="15.6" customHeight="1">
       <c r="A34" s="120"/>
       <c r="B34" s="121"/>
       <c r="C34" s="132"/>
       <c r="D34" s="133"/>
-      <c r="E34" s="288"/>
-      <c r="F34" s="289"/>
-      <c r="G34" s="285"/>
-      <c r="H34" s="286"/>
-      <c r="I34" s="287"/>
+      <c r="E34" s="296"/>
+      <c r="F34" s="297"/>
+      <c r="G34" s="293"/>
+      <c r="H34" s="294"/>
+      <c r="I34" s="295"/>
     </row>
     <row r="35" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A35" s="120"/>
       <c r="B35" s="121"/>
       <c r="C35" s="132"/>
       <c r="D35" s="133"/>
-      <c r="E35" s="288"/>
-      <c r="F35" s="289"/>
-      <c r="G35" s="285"/>
-      <c r="H35" s="286"/>
-      <c r="I35" s="287"/>
+      <c r="E35" s="296"/>
+      <c r="F35" s="297"/>
+      <c r="G35" s="293"/>
+      <c r="H35" s="294"/>
+      <c r="I35" s="295"/>
     </row>
     <row r="36" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A36" s="120"/>
       <c r="B36" s="121"/>
       <c r="C36" s="132"/>
       <c r="D36" s="133"/>
-      <c r="E36" s="288"/>
-      <c r="F36" s="289"/>
-      <c r="G36" s="285"/>
-      <c r="H36" s="286"/>
-      <c r="I36" s="287"/>
+      <c r="E36" s="296"/>
+      <c r="F36" s="297"/>
+      <c r="G36" s="293"/>
+      <c r="H36" s="294"/>
+      <c r="I36" s="295"/>
     </row>
     <row r="37" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A37" s="120"/>
       <c r="B37" s="121"/>
       <c r="C37" s="132"/>
       <c r="D37" s="133"/>
-      <c r="E37" s="288"/>
-      <c r="F37" s="289"/>
-      <c r="G37" s="285"/>
-      <c r="H37" s="286"/>
-      <c r="I37" s="287"/>
+      <c r="E37" s="296"/>
+      <c r="F37" s="297"/>
+      <c r="G37" s="293"/>
+      <c r="H37" s="294"/>
+      <c r="I37" s="295"/>
     </row>
     <row r="38" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A38" s="120"/>
       <c r="B38" s="121"/>
       <c r="C38" s="132"/>
       <c r="D38" s="133"/>
-      <c r="E38" s="288"/>
-      <c r="F38" s="289"/>
-      <c r="G38" s="285"/>
-      <c r="H38" s="286"/>
-      <c r="I38" s="287"/>
+      <c r="E38" s="296"/>
+      <c r="F38" s="297"/>
+      <c r="G38" s="293"/>
+      <c r="H38" s="294"/>
+      <c r="I38" s="295"/>
     </row>
     <row r="39" spans="1:10" s="127" customFormat="1" ht="15.6" customHeight="1">
       <c r="A39" s="120"/>
       <c r="B39" s="121"/>
       <c r="C39" s="132"/>
       <c r="D39" s="133"/>
-      <c r="E39" s="288"/>
-      <c r="F39" s="289"/>
-      <c r="G39" s="285"/>
-      <c r="H39" s="286"/>
-      <c r="I39" s="287"/>
+      <c r="E39" s="296"/>
+      <c r="F39" s="297"/>
+      <c r="G39" s="293"/>
+      <c r="H39" s="294"/>
+      <c r="I39" s="295"/>
     </row>
     <row r="40" spans="1:10" s="127" customFormat="1" ht="15.6" customHeight="1">
       <c r="A40" s="120"/>
       <c r="B40" s="121"/>
       <c r="C40" s="132"/>
       <c r="D40" s="133"/>
-      <c r="E40" s="288"/>
-      <c r="F40" s="289"/>
-      <c r="G40" s="285"/>
-      <c r="H40" s="286"/>
-      <c r="I40" s="287"/>
+      <c r="E40" s="296"/>
+      <c r="F40" s="297"/>
+      <c r="G40" s="293"/>
+      <c r="H40" s="294"/>
+      <c r="I40" s="295"/>
     </row>
     <row r="41" spans="1:10" s="127" customFormat="1" ht="15.75">
       <c r="A41" s="120"/>
       <c r="B41" s="121"/>
       <c r="C41" s="132"/>
       <c r="D41" s="133"/>
-      <c r="E41" s="288"/>
-      <c r="F41" s="289"/>
-      <c r="G41" s="285"/>
-      <c r="H41" s="286"/>
-      <c r="I41" s="287"/>
+      <c r="E41" s="296"/>
+      <c r="F41" s="297"/>
+      <c r="G41" s="293"/>
+      <c r="H41" s="294"/>
+      <c r="I41" s="295"/>
     </row>
     <row r="42" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1">
       <c r="A42" s="120"/>
@@ -7301,9 +7478,9 @@
       <c r="E47" s="252"/>
       <c r="F47" s="207"/>
       <c r="G47" s="155"/>
-      <c r="H47" s="282"/>
-      <c r="I47" s="283"/>
-      <c r="J47" s="284"/>
+      <c r="H47" s="290"/>
+      <c r="I47" s="291"/>
+      <c r="J47" s="292"/>
     </row>
     <row r="48" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A48" s="120"/>
@@ -7313,9 +7490,9 @@
       <c r="E48" s="253"/>
       <c r="F48" s="207"/>
       <c r="G48" s="155"/>
-      <c r="H48" s="282"/>
-      <c r="I48" s="283"/>
-      <c r="J48" s="284"/>
+      <c r="H48" s="290"/>
+      <c r="I48" s="291"/>
+      <c r="J48" s="292"/>
     </row>
     <row r="49" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A49" s="120"/>
@@ -7325,9 +7502,9 @@
       <c r="E49" s="254"/>
       <c r="F49" s="207"/>
       <c r="G49" s="155"/>
-      <c r="H49" s="282"/>
-      <c r="I49" s="283"/>
-      <c r="J49" s="284"/>
+      <c r="H49" s="290"/>
+      <c r="I49" s="291"/>
+      <c r="J49" s="292"/>
     </row>
     <row r="50" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A50" s="120"/>
@@ -7337,9 +7514,9 @@
       <c r="E50" s="252"/>
       <c r="F50" s="207"/>
       <c r="G50" s="155"/>
-      <c r="H50" s="282"/>
-      <c r="I50" s="283"/>
-      <c r="J50" s="284"/>
+      <c r="H50" s="290"/>
+      <c r="I50" s="291"/>
+      <c r="J50" s="292"/>
     </row>
     <row r="51" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A51" s="120"/>
@@ -7349,9 +7526,9 @@
       <c r="E51" s="252"/>
       <c r="F51" s="207"/>
       <c r="G51" s="155"/>
-      <c r="H51" s="282"/>
-      <c r="I51" s="283"/>
-      <c r="J51" s="284"/>
+      <c r="H51" s="290"/>
+      <c r="I51" s="291"/>
+      <c r="J51" s="292"/>
     </row>
     <row r="52" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A52" s="120"/>
@@ -7361,9 +7538,9 @@
       <c r="E52" s="252"/>
       <c r="F52" s="207"/>
       <c r="G52" s="155"/>
-      <c r="H52" s="282"/>
-      <c r="I52" s="283"/>
-      <c r="J52" s="284"/>
+      <c r="H52" s="290"/>
+      <c r="I52" s="291"/>
+      <c r="J52" s="292"/>
     </row>
     <row r="53" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A53" s="120"/>
@@ -7373,9 +7550,9 @@
       <c r="E53" s="253"/>
       <c r="F53" s="207"/>
       <c r="G53" s="155"/>
-      <c r="H53" s="282"/>
-      <c r="I53" s="283"/>
-      <c r="J53" s="284"/>
+      <c r="H53" s="290"/>
+      <c r="I53" s="291"/>
+      <c r="J53" s="292"/>
     </row>
     <row r="54" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A54" s="120"/>
@@ -7385,9 +7562,9 @@
       <c r="E54" s="254"/>
       <c r="F54" s="207"/>
       <c r="G54" s="155"/>
-      <c r="H54" s="282"/>
-      <c r="I54" s="283"/>
-      <c r="J54" s="284"/>
+      <c r="H54" s="290"/>
+      <c r="I54" s="291"/>
+      <c r="J54" s="292"/>
     </row>
     <row r="55" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A55" s="120"/>
@@ -7397,9 +7574,9 @@
       <c r="E55" s="252"/>
       <c r="F55" s="207"/>
       <c r="G55" s="155"/>
-      <c r="H55" s="282"/>
-      <c r="I55" s="283"/>
-      <c r="J55" s="284"/>
+      <c r="H55" s="290"/>
+      <c r="I55" s="291"/>
+      <c r="J55" s="292"/>
     </row>
     <row r="56" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A56" s="120"/>
@@ -7409,9 +7586,9 @@
       <c r="E56" s="252"/>
       <c r="F56" s="207"/>
       <c r="G56" s="155"/>
-      <c r="H56" s="282"/>
-      <c r="I56" s="283"/>
-      <c r="J56" s="284"/>
+      <c r="H56" s="290"/>
+      <c r="I56" s="291"/>
+      <c r="J56" s="292"/>
     </row>
     <row r="57" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A57" s="120"/>
@@ -7421,9 +7598,9 @@
       <c r="E57" s="252"/>
       <c r="F57" s="207"/>
       <c r="G57" s="155"/>
-      <c r="H57" s="282"/>
-      <c r="I57" s="283"/>
-      <c r="J57" s="284"/>
+      <c r="H57" s="290"/>
+      <c r="I57" s="291"/>
+      <c r="J57" s="292"/>
     </row>
     <row r="58" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A58" s="120"/>
@@ -7433,9 +7610,9 @@
       <c r="E58" s="253"/>
       <c r="F58" s="207"/>
       <c r="G58" s="155"/>
-      <c r="H58" s="282"/>
-      <c r="I58" s="283"/>
-      <c r="J58" s="284"/>
+      <c r="H58" s="290"/>
+      <c r="I58" s="291"/>
+      <c r="J58" s="292"/>
     </row>
     <row r="59" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A59" s="120"/>
@@ -7445,9 +7622,9 @@
       <c r="E59" s="254"/>
       <c r="F59" s="207"/>
       <c r="G59" s="155"/>
-      <c r="H59" s="282"/>
-      <c r="I59" s="283"/>
-      <c r="J59" s="284"/>
+      <c r="H59" s="290"/>
+      <c r="I59" s="291"/>
+      <c r="J59" s="292"/>
     </row>
     <row r="60" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A60" s="120"/>
@@ -7457,9 +7634,9 @@
       <c r="E60" s="252"/>
       <c r="F60" s="207"/>
       <c r="G60" s="155"/>
-      <c r="H60" s="282"/>
-      <c r="I60" s="283"/>
-      <c r="J60" s="284"/>
+      <c r="H60" s="290"/>
+      <c r="I60" s="291"/>
+      <c r="J60" s="292"/>
     </row>
     <row r="61" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A61" s="120"/>
@@ -7469,9 +7646,9 @@
       <c r="E61" s="252"/>
       <c r="F61" s="207"/>
       <c r="G61" s="155"/>
-      <c r="H61" s="282"/>
-      <c r="I61" s="283"/>
-      <c r="J61" s="284"/>
+      <c r="H61" s="290"/>
+      <c r="I61" s="291"/>
+      <c r="J61" s="292"/>
     </row>
     <row r="62" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A62" s="120"/>
@@ -7481,9 +7658,9 @@
       <c r="E62" s="252"/>
       <c r="F62" s="207"/>
       <c r="G62" s="155"/>
-      <c r="H62" s="282"/>
-      <c r="I62" s="283"/>
-      <c r="J62" s="284"/>
+      <c r="H62" s="290"/>
+      <c r="I62" s="291"/>
+      <c r="J62" s="292"/>
     </row>
     <row r="63" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A63" s="120"/>
@@ -7493,9 +7670,9 @@
       <c r="E63" s="253"/>
       <c r="F63" s="207"/>
       <c r="G63" s="155"/>
-      <c r="H63" s="282"/>
-      <c r="I63" s="283"/>
-      <c r="J63" s="284"/>
+      <c r="H63" s="290"/>
+      <c r="I63" s="291"/>
+      <c r="J63" s="292"/>
     </row>
     <row r="64" spans="1:10" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A64" s="120"/>
@@ -7505,9 +7682,9 @@
       <c r="E64" s="254"/>
       <c r="F64" s="207"/>
       <c r="G64" s="155"/>
-      <c r="H64" s="282"/>
-      <c r="I64" s="283"/>
-      <c r="J64" s="284"/>
+      <c r="H64" s="290"/>
+      <c r="I64" s="291"/>
+      <c r="J64" s="292"/>
     </row>
     <row r="65" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A65" s="120"/>
@@ -7517,9 +7694,9 @@
       <c r="E65" s="252"/>
       <c r="F65" s="207"/>
       <c r="G65" s="155"/>
-      <c r="H65" s="282"/>
-      <c r="I65" s="283"/>
-      <c r="J65" s="284"/>
+      <c r="H65" s="290"/>
+      <c r="I65" s="291"/>
+      <c r="J65" s="292"/>
     </row>
     <row r="66" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A66" s="120"/>
@@ -7529,9 +7706,9 @@
       <c r="E66" s="252"/>
       <c r="F66" s="207"/>
       <c r="G66" s="155"/>
-      <c r="H66" s="282"/>
-      <c r="I66" s="283"/>
-      <c r="J66" s="284"/>
+      <c r="H66" s="290"/>
+      <c r="I66" s="291"/>
+      <c r="J66" s="292"/>
     </row>
     <row r="67" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="120"/>
@@ -7541,9 +7718,9 @@
       <c r="E67" s="252"/>
       <c r="F67" s="207"/>
       <c r="G67" s="155"/>
-      <c r="H67" s="282"/>
-      <c r="I67" s="283"/>
-      <c r="J67" s="284"/>
+      <c r="H67" s="290"/>
+      <c r="I67" s="291"/>
+      <c r="J67" s="292"/>
     </row>
     <row r="68" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A68" s="120"/>
@@ -7553,9 +7730,9 @@
       <c r="E68" s="253"/>
       <c r="F68" s="207"/>
       <c r="G68" s="155"/>
-      <c r="H68" s="282"/>
-      <c r="I68" s="283"/>
-      <c r="J68" s="284"/>
+      <c r="H68" s="290"/>
+      <c r="I68" s="291"/>
+      <c r="J68" s="292"/>
     </row>
     <row r="69" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="120"/>
@@ -7565,9 +7742,9 @@
       <c r="E69" s="254"/>
       <c r="F69" s="207"/>
       <c r="G69" s="155"/>
-      <c r="H69" s="282"/>
-      <c r="I69" s="283"/>
-      <c r="J69" s="284"/>
+      <c r="H69" s="290"/>
+      <c r="I69" s="291"/>
+      <c r="J69" s="292"/>
     </row>
     <row r="70" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A70" s="120"/>
@@ -7577,9 +7754,9 @@
       <c r="E70" s="252"/>
       <c r="F70" s="207"/>
       <c r="G70" s="155"/>
-      <c r="H70" s="282"/>
-      <c r="I70" s="283"/>
-      <c r="J70" s="284"/>
+      <c r="H70" s="290"/>
+      <c r="I70" s="291"/>
+      <c r="J70" s="292"/>
     </row>
     <row r="71" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="120"/>
@@ -7589,9 +7766,9 @@
       <c r="E71" s="252"/>
       <c r="F71" s="207"/>
       <c r="G71" s="155"/>
-      <c r="H71" s="282"/>
-      <c r="I71" s="283"/>
-      <c r="J71" s="284"/>
+      <c r="H71" s="290"/>
+      <c r="I71" s="291"/>
+      <c r="J71" s="292"/>
     </row>
     <row r="72" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A72" s="120"/>
@@ -7601,9 +7778,9 @@
       <c r="E72" s="252"/>
       <c r="F72" s="207"/>
       <c r="G72" s="155"/>
-      <c r="H72" s="282"/>
-      <c r="I72" s="283"/>
-      <c r="J72" s="284"/>
+      <c r="H72" s="290"/>
+      <c r="I72" s="291"/>
+      <c r="J72" s="292"/>
     </row>
     <row r="73" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="120"/>
@@ -7613,9 +7790,9 @@
       <c r="E73" s="253"/>
       <c r="F73" s="207"/>
       <c r="G73" s="155"/>
-      <c r="H73" s="282"/>
-      <c r="I73" s="283"/>
-      <c r="J73" s="284"/>
+      <c r="H73" s="290"/>
+      <c r="I73" s="291"/>
+      <c r="J73" s="292"/>
     </row>
     <row r="74" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A74" s="120"/>
@@ -7625,9 +7802,9 @@
       <c r="E74" s="254"/>
       <c r="F74" s="207"/>
       <c r="G74" s="155"/>
-      <c r="H74" s="282"/>
-      <c r="I74" s="283"/>
-      <c r="J74" s="284"/>
+      <c r="H74" s="290"/>
+      <c r="I74" s="291"/>
+      <c r="J74" s="292"/>
     </row>
     <row r="75" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A75" s="120"/>
@@ -7637,9 +7814,9 @@
       <c r="E75" s="252"/>
       <c r="F75" s="207"/>
       <c r="G75" s="155"/>
-      <c r="H75" s="282"/>
-      <c r="I75" s="283"/>
-      <c r="J75" s="284"/>
+      <c r="H75" s="290"/>
+      <c r="I75" s="291"/>
+      <c r="J75" s="292"/>
     </row>
     <row r="76" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A76" s="120"/>
@@ -7649,9 +7826,9 @@
       <c r="E76" s="252"/>
       <c r="F76" s="207"/>
       <c r="G76" s="155"/>
-      <c r="H76" s="282"/>
-      <c r="I76" s="283"/>
-      <c r="J76" s="284"/>
+      <c r="H76" s="290"/>
+      <c r="I76" s="291"/>
+      <c r="J76" s="292"/>
     </row>
     <row r="77" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A77" s="120"/>
@@ -7661,9 +7838,9 @@
       <c r="E77" s="252"/>
       <c r="F77" s="207"/>
       <c r="G77" s="155"/>
-      <c r="H77" s="282"/>
-      <c r="I77" s="283"/>
-      <c r="J77" s="284"/>
+      <c r="H77" s="290"/>
+      <c r="I77" s="291"/>
+      <c r="J77" s="292"/>
     </row>
     <row r="78" spans="1:11" s="127" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A78" s="120"/>
@@ -7673,9 +7850,9 @@
       <c r="E78" s="253"/>
       <c r="F78" s="207"/>
       <c r="G78" s="155"/>
-      <c r="H78" s="282"/>
-      <c r="I78" s="283"/>
-      <c r="J78" s="284"/>
+      <c r="H78" s="290"/>
+      <c r="I78" s="291"/>
+      <c r="J78" s="292"/>
     </row>
     <row r="79" spans="1:11" s="119" customFormat="1" ht="4.5" customHeight="1">
       <c r="A79" s="111"/>
@@ -7708,67 +7885,16 @@
       <c r="A81" s="111"/>
       <c r="B81" s="166"/>
       <c r="C81" s="167"/>
-      <c r="D81" s="299"/>
-      <c r="E81" s="300"/>
-      <c r="F81" s="300"/>
-      <c r="G81" s="300"/>
-      <c r="H81" s="300"/>
-      <c r="I81" s="300"/>
-      <c r="J81" s="301"/>
+      <c r="D81" s="287"/>
+      <c r="E81" s="288"/>
+      <c r="F81" s="288"/>
+      <c r="G81" s="288"/>
+      <c r="H81" s="288"/>
+      <c r="I81" s="288"/>
+      <c r="J81" s="289"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="D81:J81"/>
-    <mergeCell ref="H77:J77"/>
-    <mergeCell ref="H78:J78"/>
-    <mergeCell ref="H75:J75"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="H74:J74"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="H69:J69"/>
-    <mergeCell ref="H70:J70"/>
-    <mergeCell ref="H67:J67"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="H65:J65"/>
-    <mergeCell ref="H66:J66"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="H59:J59"/>
-    <mergeCell ref="H60:J60"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="H58:J58"/>
-    <mergeCell ref="H55:J55"/>
-    <mergeCell ref="H56:J56"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="G33:I33"/>
     <mergeCell ref="G34:I34"/>
@@ -7781,6 +7907,57 @@
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="G32:I32"/>
     <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="H55:J55"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="H59:J59"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="H67:J67"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="H74:J74"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="H69:J69"/>
+    <mergeCell ref="H70:J70"/>
+    <mergeCell ref="D81:J81"/>
+    <mergeCell ref="H77:J77"/>
+    <mergeCell ref="H78:J78"/>
+    <mergeCell ref="H75:J75"/>
+    <mergeCell ref="H76:J76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -7799,10 +7976,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -7810,7 +7987,7 @@
     <col min="1" max="1" width="7.140625" style="211" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="209" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="209" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="210" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="210" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="211" customWidth="1"/>
     <col min="6" max="7" width="13.140625" style="212" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" style="239" customWidth="1"/>
@@ -7867,7 +8044,7 @@
       <c r="A3" s="211" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="305" t="s">
+      <c r="B3" s="307" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="217" t="s">
@@ -7877,7 +8054,7 @@
         <v>74</v>
       </c>
       <c r="E3" s="245" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F3" s="219"/>
       <c r="G3" s="219"/>
@@ -7888,16 +8065,16 @@
       <c r="J3" s="220">
         <v>42057</v>
       </c>
-      <c r="K3" s="308" t="s">
-        <v>103</v>
+      <c r="K3" s="310" t="s">
+        <v>100</v>
       </c>
       <c r="L3" s="218" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M3" s="221"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B4" s="306"/>
+      <c r="B4" s="308"/>
       <c r="C4" s="229" t="s">
         <v>73</v>
       </c>
@@ -7905,515 +8082,545 @@
         <v>75</v>
       </c>
       <c r="E4" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F4" s="256"/>
       <c r="G4" s="256"/>
       <c r="H4" s="243"/>
-      <c r="I4" s="311">
+      <c r="I4" s="268">
         <v>42050</v>
       </c>
-      <c r="J4" s="311">
+      <c r="J4" s="268">
         <v>42057</v>
       </c>
-      <c r="K4" s="309"/>
+      <c r="K4" s="311"/>
       <c r="L4" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M4" s="233"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B5" s="306"/>
+      <c r="B5" s="308"/>
       <c r="C5" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D5" s="230" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="E5" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F5" s="256"/>
       <c r="G5" s="256"/>
       <c r="H5" s="243"/>
-      <c r="I5" s="311">
+      <c r="I5" s="268">
         <v>42050</v>
       </c>
-      <c r="J5" s="311">
+      <c r="J5" s="268">
         <v>42057</v>
       </c>
-      <c r="K5" s="309"/>
+      <c r="K5" s="311"/>
       <c r="L5" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M5" s="233"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B6" s="306"/>
+      <c r="B6" s="308"/>
       <c r="C6" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="235" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="E6" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F6" s="262"/>
       <c r="G6" s="262"/>
       <c r="H6" s="244"/>
-      <c r="I6" s="311">
+      <c r="I6" s="268">
         <v>42050</v>
       </c>
-      <c r="J6" s="311">
+      <c r="J6" s="268">
         <v>42057</v>
       </c>
-      <c r="K6" s="309"/>
+      <c r="K6" s="311"/>
       <c r="L6" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M6" s="238"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B7" s="306"/>
+      <c r="B7" s="308"/>
       <c r="C7" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="230" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="E7" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F7" s="256"/>
       <c r="G7" s="256"/>
       <c r="H7" s="243"/>
-      <c r="I7" s="311">
+      <c r="I7" s="268">
         <v>42050</v>
       </c>
-      <c r="J7" s="311">
+      <c r="J7" s="268">
         <v>42057</v>
       </c>
-      <c r="K7" s="309"/>
+      <c r="K7" s="311"/>
       <c r="L7" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M7" s="233"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B8" s="306"/>
+      <c r="B8" s="308"/>
       <c r="C8" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="230" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E8" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F8" s="256"/>
       <c r="G8" s="256"/>
       <c r="H8" s="243"/>
-      <c r="I8" s="311">
+      <c r="I8" s="268">
         <v>42050</v>
       </c>
-      <c r="J8" s="311">
+      <c r="J8" s="268">
         <v>42057</v>
       </c>
-      <c r="K8" s="309"/>
+      <c r="K8" s="311"/>
       <c r="L8" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M8" s="233"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B9" s="306"/>
+      <c r="B9" s="308"/>
       <c r="C9" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="230" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E9" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F9" s="231"/>
       <c r="G9" s="231"/>
       <c r="H9" s="243"/>
-      <c r="I9" s="311">
+      <c r="I9" s="268">
         <v>42050</v>
       </c>
-      <c r="J9" s="311">
+      <c r="J9" s="268">
         <v>42057</v>
       </c>
-      <c r="K9" s="309"/>
+      <c r="K9" s="311"/>
       <c r="L9" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M9" s="233"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B10" s="306"/>
+      <c r="B10" s="308"/>
       <c r="C10" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D10" s="230" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E10" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F10" s="231"/>
       <c r="G10" s="231"/>
       <c r="H10" s="243"/>
-      <c r="I10" s="311">
+      <c r="I10" s="268">
         <v>42050</v>
       </c>
-      <c r="J10" s="311">
+      <c r="J10" s="268">
         <v>42057</v>
       </c>
-      <c r="K10" s="309"/>
+      <c r="K10" s="311"/>
       <c r="L10" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M10" s="233"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B11" s="306"/>
+      <c r="B11" s="308"/>
       <c r="C11" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="230" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E11" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F11" s="231"/>
       <c r="G11" s="231"/>
       <c r="H11" s="243"/>
-      <c r="I11" s="311">
+      <c r="I11" s="268">
         <v>42050</v>
       </c>
-      <c r="J11" s="311">
+      <c r="J11" s="268">
         <v>42057</v>
       </c>
-      <c r="K11" s="309"/>
+      <c r="K11" s="311"/>
       <c r="L11" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M11" s="233"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B12" s="306"/>
+      <c r="B12" s="308"/>
       <c r="C12" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="230" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E12" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F12" s="231"/>
       <c r="G12" s="231"/>
       <c r="H12" s="243"/>
-      <c r="I12" s="311">
+      <c r="I12" s="268">
         <v>42050</v>
       </c>
-      <c r="J12" s="311">
+      <c r="J12" s="268">
         <v>42057</v>
       </c>
-      <c r="K12" s="309"/>
+      <c r="K12" s="311"/>
       <c r="L12" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M12" s="233"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B13" s="306"/>
+      <c r="B13" s="308"/>
       <c r="C13" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D13" s="230" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E13" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F13" s="231"/>
       <c r="G13" s="231"/>
       <c r="H13" s="243"/>
-      <c r="I13" s="311">
+      <c r="I13" s="268">
         <v>42050</v>
       </c>
-      <c r="J13" s="311">
+      <c r="J13" s="268">
         <v>42057</v>
       </c>
-      <c r="K13" s="309"/>
+      <c r="K13" s="311"/>
       <c r="L13" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M13" s="233"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B14" s="306"/>
+      <c r="B14" s="308"/>
       <c r="C14" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D14" s="230" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E14" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F14" s="231"/>
       <c r="G14" s="231"/>
       <c r="H14" s="243"/>
-      <c r="I14" s="311">
+      <c r="I14" s="268">
         <v>42050</v>
       </c>
-      <c r="J14" s="311">
+      <c r="J14" s="268">
         <v>42057</v>
       </c>
-      <c r="K14" s="309"/>
+      <c r="K14" s="311"/>
       <c r="L14" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M14" s="233"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B15" s="306"/>
+      <c r="B15" s="308"/>
       <c r="C15" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="230" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E15" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F15" s="231"/>
       <c r="G15" s="231"/>
       <c r="H15" s="243"/>
-      <c r="I15" s="311">
+      <c r="I15" s="268">
         <v>42050</v>
       </c>
-      <c r="J15" s="311">
+      <c r="J15" s="268">
         <v>42057</v>
       </c>
-      <c r="K15" s="309"/>
+      <c r="K15" s="311"/>
       <c r="L15" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M15" s="233"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B16" s="306"/>
+      <c r="B16" s="308"/>
       <c r="C16" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D16" s="230" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E16" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F16" s="231"/>
       <c r="G16" s="231"/>
       <c r="H16" s="243"/>
-      <c r="I16" s="311">
+      <c r="I16" s="268">
         <v>42050</v>
       </c>
-      <c r="J16" s="311">
+      <c r="J16" s="268">
         <v>42057</v>
       </c>
-      <c r="K16" s="309"/>
+      <c r="K16" s="311"/>
       <c r="L16" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M16" s="233"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B17" s="306"/>
+      <c r="B17" s="308"/>
       <c r="C17" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D17" s="230" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E17" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F17" s="231"/>
       <c r="G17" s="231"/>
       <c r="H17" s="243"/>
-      <c r="I17" s="311">
+      <c r="I17" s="268">
         <v>42050</v>
       </c>
-      <c r="J17" s="311">
+      <c r="J17" s="268">
         <v>42057</v>
       </c>
-      <c r="K17" s="309"/>
+      <c r="K17" s="311"/>
       <c r="L17" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M17" s="233"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B18" s="306"/>
+      <c r="B18" s="308"/>
       <c r="C18" s="229" t="s">
         <v>73</v>
       </c>
       <c r="D18" s="230" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="E18" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F18" s="231"/>
       <c r="G18" s="231"/>
       <c r="H18" s="243"/>
-      <c r="I18" s="311">
+      <c r="I18" s="268">
         <v>42050</v>
       </c>
-      <c r="J18" s="311">
+      <c r="J18" s="268">
         <v>42057</v>
       </c>
-      <c r="K18" s="309"/>
+      <c r="K18" s="311"/>
       <c r="L18" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M18" s="233"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B19" s="306"/>
+      <c r="B19" s="308"/>
       <c r="C19" s="229" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D19" s="230" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="E19" s="247" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F19" s="231"/>
       <c r="G19" s="231"/>
       <c r="H19" s="243"/>
-      <c r="I19" s="311">
+      <c r="I19" s="268">
         <v>42050</v>
       </c>
-      <c r="J19" s="311">
+      <c r="J19" s="268">
         <v>42057</v>
       </c>
-      <c r="K19" s="309"/>
+      <c r="K19" s="311"/>
       <c r="L19" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M19" s="233"/>
     </row>
     <row r="20" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B20" s="306"/>
+      <c r="B20" s="308"/>
       <c r="C20" s="229" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D20" s="230" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E20" s="247" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F20" s="231"/>
       <c r="G20" s="231"/>
       <c r="H20" s="243"/>
-      <c r="I20" s="311">
+      <c r="I20" s="268">
         <v>42050</v>
       </c>
-      <c r="J20" s="311">
+      <c r="J20" s="268">
         <v>42057</v>
       </c>
-      <c r="K20" s="310"/>
+      <c r="K20" s="311"/>
       <c r="L20" s="230" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M20" s="233"/>
     </row>
     <row r="21" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B21" s="306"/>
+      <c r="B21" s="308"/>
       <c r="C21" s="229" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="D21" s="230" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="E21" s="247" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="256">
-        <v>42060</v>
-      </c>
-      <c r="G21" s="256">
-        <v>42063</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F21" s="231"/>
+      <c r="G21" s="231"/>
       <c r="H21" s="243"/>
-      <c r="I21" s="311"/>
-      <c r="J21" s="311"/>
-      <c r="K21" s="243"/>
-      <c r="L21" s="230"/>
+      <c r="I21" s="268">
+        <v>42050</v>
+      </c>
+      <c r="J21" s="268">
+        <v>42057</v>
+      </c>
+      <c r="K21" s="311"/>
+      <c r="L21" s="230" t="s">
+        <v>99</v>
+      </c>
       <c r="M21" s="233"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B22" s="306"/>
+      <c r="B22" s="308"/>
       <c r="C22" s="229" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="230" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="230"/>
-      <c r="E22" s="247"/>
+      <c r="E22" s="247" t="s">
+        <v>95</v>
+      </c>
       <c r="F22" s="231"/>
       <c r="G22" s="231"/>
       <c r="H22" s="243"/>
-      <c r="I22" s="232"/>
-      <c r="J22" s="232"/>
-      <c r="K22" s="243"/>
-      <c r="L22" s="230"/>
+      <c r="I22" s="268">
+        <v>42050</v>
+      </c>
+      <c r="J22" s="268">
+        <v>42057</v>
+      </c>
+      <c r="K22" s="311"/>
+      <c r="L22" s="230" t="s">
+        <v>99</v>
+      </c>
       <c r="M22" s="233"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B23" s="306"/>
+      <c r="B23" s="308"/>
       <c r="C23" s="229" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="230"/>
-      <c r="E23" s="247"/>
+        <v>93</v>
+      </c>
+      <c r="D23" s="230" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="247" t="s">
+        <v>98</v>
+      </c>
       <c r="F23" s="231"/>
       <c r="G23" s="231"/>
       <c r="H23" s="243"/>
-      <c r="I23" s="232"/>
-      <c r="J23" s="232"/>
-      <c r="K23" s="243"/>
-      <c r="L23" s="230"/>
+      <c r="I23" s="268">
+        <v>42050</v>
+      </c>
+      <c r="J23" s="268">
+        <v>42057</v>
+      </c>
+      <c r="K23" s="312"/>
+      <c r="L23" s="230" t="s">
+        <v>99</v>
+      </c>
       <c r="M23" s="233"/>
     </row>
     <row r="24" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B24" s="306"/>
+      <c r="B24" s="308"/>
       <c r="C24" s="229" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="230"/>
-      <c r="E24" s="247"/>
-      <c r="F24" s="231"/>
-      <c r="G24" s="231"/>
+        <v>104</v>
+      </c>
+      <c r="D24" s="230" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="247" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="256">
+        <v>42060</v>
+      </c>
+      <c r="G24" s="256">
+        <v>42063</v>
+      </c>
       <c r="H24" s="243"/>
-      <c r="I24" s="232"/>
-      <c r="J24" s="232"/>
+      <c r="I24" s="268"/>
+      <c r="J24" s="268"/>
       <c r="K24" s="243"/>
       <c r="L24" s="230"/>
       <c r="M24" s="233"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B25" s="306"/>
+      <c r="B25" s="308"/>
       <c r="C25" s="229" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D25" s="230"/>
       <c r="E25" s="247"/>
@@ -8427,25 +8634,35 @@
       <c r="M25" s="233"/>
     </row>
     <row r="26" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B26" s="306"/>
+      <c r="B26" s="308"/>
       <c r="C26" s="229" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="230"/>
-      <c r="E26" s="247"/>
+        <v>96</v>
+      </c>
+      <c r="D26" s="230" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="247" t="s">
+        <v>95</v>
+      </c>
       <c r="F26" s="231"/>
       <c r="G26" s="231"/>
       <c r="H26" s="243"/>
-      <c r="I26" s="232"/>
-      <c r="J26" s="232"/>
+      <c r="I26" s="268">
+        <v>42058</v>
+      </c>
+      <c r="J26" s="268">
+        <v>42067</v>
+      </c>
       <c r="K26" s="243"/>
-      <c r="L26" s="230"/>
+      <c r="L26" s="230" t="s">
+        <v>99</v>
+      </c>
       <c r="M26" s="233"/>
     </row>
     <row r="27" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B27" s="306"/>
+      <c r="B27" s="308"/>
       <c r="C27" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D27" s="230"/>
       <c r="E27" s="247"/>
@@ -8459,9 +8676,9 @@
       <c r="M27" s="233"/>
     </row>
     <row r="28" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B28" s="306"/>
+      <c r="B28" s="308"/>
       <c r="C28" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D28" s="230"/>
       <c r="E28" s="247"/>
@@ -8475,9 +8692,9 @@
       <c r="M28" s="233"/>
     </row>
     <row r="29" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B29" s="306"/>
+      <c r="B29" s="308"/>
       <c r="C29" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D29" s="230"/>
       <c r="E29" s="247"/>
@@ -8491,9 +8708,9 @@
       <c r="M29" s="233"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B30" s="306"/>
+      <c r="B30" s="308"/>
       <c r="C30" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D30" s="230"/>
       <c r="E30" s="247"/>
@@ -8507,9 +8724,9 @@
       <c r="M30" s="233"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B31" s="306"/>
+      <c r="B31" s="308"/>
       <c r="C31" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D31" s="230"/>
       <c r="E31" s="247"/>
@@ -8523,9 +8740,9 @@
       <c r="M31" s="233"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B32" s="306"/>
+      <c r="B32" s="308"/>
       <c r="C32" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D32" s="230"/>
       <c r="E32" s="247"/>
@@ -8539,9 +8756,9 @@
       <c r="M32" s="233"/>
     </row>
     <row r="33" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B33" s="306"/>
+      <c r="B33" s="308"/>
       <c r="C33" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D33" s="230"/>
       <c r="E33" s="247"/>
@@ -8555,9 +8772,9 @@
       <c r="M33" s="233"/>
     </row>
     <row r="34" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B34" s="306"/>
+      <c r="B34" s="308"/>
       <c r="C34" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D34" s="230"/>
       <c r="E34" s="247"/>
@@ -8571,9 +8788,9 @@
       <c r="M34" s="233"/>
     </row>
     <row r="35" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B35" s="306"/>
+      <c r="B35" s="308"/>
       <c r="C35" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D35" s="230"/>
       <c r="E35" s="247"/>
@@ -8587,9 +8804,9 @@
       <c r="M35" s="233"/>
     </row>
     <row r="36" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B36" s="306"/>
+      <c r="B36" s="308"/>
       <c r="C36" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D36" s="230"/>
       <c r="E36" s="247"/>
@@ -8603,9 +8820,9 @@
       <c r="M36" s="233"/>
     </row>
     <row r="37" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B37" s="306"/>
+      <c r="B37" s="308"/>
       <c r="C37" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D37" s="230"/>
       <c r="E37" s="247"/>
@@ -8619,9 +8836,9 @@
       <c r="M37" s="233"/>
     </row>
     <row r="38" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B38" s="306"/>
+      <c r="B38" s="308"/>
       <c r="C38" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D38" s="230"/>
       <c r="E38" s="247"/>
@@ -8635,9 +8852,9 @@
       <c r="M38" s="233"/>
     </row>
     <row r="39" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B39" s="306"/>
+      <c r="B39" s="308"/>
       <c r="C39" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D39" s="230"/>
       <c r="E39" s="247"/>
@@ -8651,9 +8868,9 @@
       <c r="M39" s="233"/>
     </row>
     <row r="40" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B40" s="306"/>
+      <c r="B40" s="308"/>
       <c r="C40" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D40" s="230"/>
       <c r="E40" s="247"/>
@@ -8667,9 +8884,9 @@
       <c r="M40" s="233"/>
     </row>
     <row r="41" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B41" s="306"/>
+      <c r="B41" s="308"/>
       <c r="C41" s="229" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D41" s="230"/>
       <c r="E41" s="247"/>
@@ -8682,39 +8899,43 @@
       <c r="L41" s="230"/>
       <c r="M41" s="233"/>
     </row>
-    <row r="42" spans="2:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B42" s="307"/>
-      <c r="C42" s="222"/>
-      <c r="D42" s="223"/>
-      <c r="E42" s="246"/>
-      <c r="F42" s="224"/>
-      <c r="G42" s="224"/>
-      <c r="H42" s="242"/>
-      <c r="I42" s="225"/>
-      <c r="J42" s="225"/>
-      <c r="K42" s="242"/>
-      <c r="L42" s="223"/>
-      <c r="M42" s="226"/>
-    </row>
-    <row r="43" spans="2:13" ht="15.75" customHeight="1" thickTop="1">
-      <c r="B43" s="264"/>
-      <c r="C43" s="217" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" s="218"/>
-      <c r="E43" s="245"/>
-      <c r="F43" s="227"/>
-      <c r="G43" s="227"/>
-      <c r="H43" s="241"/>
-      <c r="I43" s="228"/>
-      <c r="J43" s="228"/>
-      <c r="K43" s="241"/>
-      <c r="L43" s="218"/>
-      <c r="M43" s="221"/>
+    <row r="42" spans="2:13" ht="15.75" customHeight="1">
+      <c r="B42" s="308"/>
+      <c r="C42" s="229" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="230"/>
+      <c r="E42" s="247"/>
+      <c r="F42" s="231"/>
+      <c r="G42" s="231"/>
+      <c r="H42" s="243"/>
+      <c r="I42" s="232"/>
+      <c r="J42" s="232"/>
+      <c r="K42" s="243"/>
+      <c r="L42" s="230"/>
+      <c r="M42" s="233"/>
+    </row>
+    <row r="43" spans="2:13" ht="15.75" customHeight="1">
+      <c r="B43" s="308"/>
+      <c r="C43" s="229" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="230"/>
+      <c r="E43" s="247"/>
+      <c r="F43" s="231"/>
+      <c r="G43" s="231"/>
+      <c r="H43" s="243"/>
+      <c r="I43" s="232"/>
+      <c r="J43" s="232"/>
+      <c r="K43" s="243"/>
+      <c r="L43" s="230"/>
+      <c r="M43" s="233"/>
     </row>
     <row r="44" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B44" s="265"/>
-      <c r="C44" s="229"/>
+      <c r="B44" s="308"/>
+      <c r="C44" s="229" t="s">
+        <v>96</v>
+      </c>
       <c r="D44" s="230"/>
       <c r="E44" s="247"/>
       <c r="F44" s="231"/>
@@ -8727,7 +8948,7 @@
       <c r="M44" s="233"/>
     </row>
     <row r="45" spans="2:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B45" s="266"/>
+      <c r="B45" s="309"/>
       <c r="C45" s="222"/>
       <c r="D45" s="223"/>
       <c r="E45" s="246"/>
@@ -8741,20 +8962,20 @@
       <c r="M45" s="226"/>
     </row>
     <row r="46" spans="2:13" ht="15.75" customHeight="1" thickTop="1">
-      <c r="B46" s="267"/>
-      <c r="C46" s="234" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="235"/>
-      <c r="E46" s="248"/>
-      <c r="F46" s="236"/>
-      <c r="G46" s="236"/>
-      <c r="H46" s="244"/>
-      <c r="I46" s="237"/>
-      <c r="J46" s="237"/>
-      <c r="K46" s="244"/>
-      <c r="L46" s="235"/>
-      <c r="M46" s="238"/>
+      <c r="B46" s="264"/>
+      <c r="C46" s="217" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="218"/>
+      <c r="E46" s="245"/>
+      <c r="F46" s="227"/>
+      <c r="G46" s="227"/>
+      <c r="H46" s="241"/>
+      <c r="I46" s="228"/>
+      <c r="J46" s="228"/>
+      <c r="K46" s="241"/>
+      <c r="L46" s="218"/>
+      <c r="M46" s="221"/>
     </row>
     <row r="47" spans="2:13" ht="15.75" customHeight="1">
       <c r="B47" s="265"/>
@@ -8770,33 +8991,35 @@
       <c r="L47" s="230"/>
       <c r="M47" s="233"/>
     </row>
-    <row r="48" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B48" s="265"/>
-      <c r="C48" s="229"/>
-      <c r="D48" s="230"/>
-      <c r="E48" s="247"/>
-      <c r="F48" s="231"/>
-      <c r="G48" s="231"/>
-      <c r="H48" s="243"/>
-      <c r="I48" s="232"/>
-      <c r="J48" s="232"/>
-      <c r="K48" s="243"/>
-      <c r="L48" s="230"/>
-      <c r="M48" s="233"/>
-    </row>
-    <row r="49" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B49" s="265"/>
-      <c r="C49" s="229"/>
-      <c r="D49" s="230"/>
-      <c r="E49" s="247"/>
-      <c r="F49" s="231"/>
-      <c r="G49" s="231"/>
-      <c r="H49" s="243"/>
-      <c r="I49" s="232"/>
-      <c r="J49" s="232"/>
-      <c r="K49" s="243"/>
-      <c r="L49" s="230"/>
-      <c r="M49" s="233"/>
+    <row r="48" spans="2:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B48" s="266"/>
+      <c r="C48" s="222"/>
+      <c r="D48" s="223"/>
+      <c r="E48" s="246"/>
+      <c r="F48" s="224"/>
+      <c r="G48" s="224"/>
+      <c r="H48" s="242"/>
+      <c r="I48" s="225"/>
+      <c r="J48" s="225"/>
+      <c r="K48" s="242"/>
+      <c r="L48" s="223"/>
+      <c r="M48" s="226"/>
+    </row>
+    <row r="49" spans="2:13" ht="15.75" customHeight="1" thickTop="1">
+      <c r="B49" s="267"/>
+      <c r="C49" s="234" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="235"/>
+      <c r="E49" s="248"/>
+      <c r="F49" s="236"/>
+      <c r="G49" s="236"/>
+      <c r="H49" s="244"/>
+      <c r="I49" s="237"/>
+      <c r="J49" s="237"/>
+      <c r="K49" s="244"/>
+      <c r="L49" s="235"/>
+      <c r="M49" s="238"/>
     </row>
     <row r="50" spans="2:13" ht="15.75" customHeight="1">
       <c r="B50" s="265"/>
@@ -8812,88 +9035,130 @@
       <c r="L50" s="230"/>
       <c r="M50" s="233"/>
     </row>
-    <row r="51" spans="2:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B51" s="266"/>
-      <c r="C51" s="222"/>
-      <c r="D51" s="223"/>
-      <c r="E51" s="246"/>
-      <c r="F51" s="224"/>
-      <c r="G51" s="224"/>
-      <c r="H51" s="242"/>
-      <c r="I51" s="225"/>
-      <c r="J51" s="225"/>
-      <c r="K51" s="242"/>
-      <c r="L51" s="223"/>
-      <c r="M51" s="226"/>
-    </row>
-    <row r="52" spans="2:13" ht="12.75" thickTop="1"/>
+    <row r="51" spans="2:13" ht="15.75" customHeight="1">
+      <c r="B51" s="265"/>
+      <c r="C51" s="229"/>
+      <c r="D51" s="230"/>
+      <c r="E51" s="247"/>
+      <c r="F51" s="231"/>
+      <c r="G51" s="231"/>
+      <c r="H51" s="243"/>
+      <c r="I51" s="232"/>
+      <c r="J51" s="232"/>
+      <c r="K51" s="243"/>
+      <c r="L51" s="230"/>
+      <c r="M51" s="233"/>
+    </row>
+    <row r="52" spans="2:13" ht="15.75" customHeight="1">
+      <c r="B52" s="265"/>
+      <c r="C52" s="229"/>
+      <c r="D52" s="230"/>
+      <c r="E52" s="247"/>
+      <c r="F52" s="231"/>
+      <c r="G52" s="231"/>
+      <c r="H52" s="243"/>
+      <c r="I52" s="232"/>
+      <c r="J52" s="232"/>
+      <c r="K52" s="243"/>
+      <c r="L52" s="230"/>
+      <c r="M52" s="233"/>
+    </row>
+    <row r="53" spans="2:13" ht="15.75" customHeight="1">
+      <c r="B53" s="265"/>
+      <c r="C53" s="229"/>
+      <c r="D53" s="230"/>
+      <c r="E53" s="247"/>
+      <c r="F53" s="231"/>
+      <c r="G53" s="231"/>
+      <c r="H53" s="243"/>
+      <c r="I53" s="232"/>
+      <c r="J53" s="232"/>
+      <c r="K53" s="243"/>
+      <c r="L53" s="230"/>
+      <c r="M53" s="233"/>
+    </row>
+    <row r="54" spans="2:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B54" s="266"/>
+      <c r="C54" s="222"/>
+      <c r="D54" s="223"/>
+      <c r="E54" s="246"/>
+      <c r="F54" s="224"/>
+      <c r="G54" s="224"/>
+      <c r="H54" s="242"/>
+      <c r="I54" s="225"/>
+      <c r="J54" s="225"/>
+      <c r="K54" s="242"/>
+      <c r="L54" s="223"/>
+      <c r="M54" s="226"/>
+    </row>
+    <row r="55" spans="2:13" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:B42"/>
-    <mergeCell ref="K3:K20"/>
+    <mergeCell ref="B3:B45"/>
+    <mergeCell ref="K3:K23"/>
   </mergeCells>
   <conditionalFormatting sqref="L1:L1048576">
     <cfRule type="cellIs" priority="18" operator="equal">
       <formula>"Delay"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L137">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+  <conditionalFormatting sqref="L3:L140">
+    <cfRule type="cellIs" dxfId="36" priority="17" operator="equal">
       <formula>"Delay"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L104">
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+  <conditionalFormatting sqref="L3:L107">
+    <cfRule type="cellIs" dxfId="35" priority="16" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="15" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"All"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"Yu"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>"Hu"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"Wang"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"Pan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"Gao"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:G5">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"All"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"Yu"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"Hu"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"Wang"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"Pan"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"Gao"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L129">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L132">
       <formula1>"进行中,已完成,Delay"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
@@ -8943,14 +9208,14 @@
     </row>
     <row r="2" spans="1:12" ht="16.5" thickTop="1">
       <c r="A2" s="172"/>
-      <c r="B2" s="302" t="s">
+      <c r="B2" s="313" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="303"/>
-      <c r="D2" s="303"/>
-      <c r="E2" s="303"/>
-      <c r="F2" s="303"/>
-      <c r="G2" s="304"/>
+      <c r="C2" s="314"/>
+      <c r="D2" s="314"/>
+      <c r="E2" s="314"/>
+      <c r="F2" s="314"/>
+      <c r="G2" s="315"/>
       <c r="H2" s="199"/>
       <c r="I2" s="199"/>
       <c r="J2" s="199"/>
@@ -9265,69 +9530,69 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="6.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" style="318" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" style="272" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="316" customFormat="1">
-      <c r="B2" s="312" t="s">
+    <row r="2" spans="2:7" s="270" customFormat="1">
+      <c r="B2" s="269" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="319" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="320"/>
-      <c r="E2" s="313" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="314"/>
-      <c r="G2" s="315"/>
+      <c r="C2" s="316" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="317"/>
+      <c r="E2" s="318" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="319"/>
+      <c r="G2" s="320"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1">
-      <c r="B3" s="317">
+      <c r="B3" s="271">
         <v>1</v>
       </c>
       <c r="C3" s="321" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D3" s="322"/>
-      <c r="E3" s="282"/>
-      <c r="F3" s="283"/>
-      <c r="G3" s="284"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="291"/>
+      <c r="G3" s="292"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="317"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="289"/>
-      <c r="E4" s="282"/>
-      <c r="F4" s="283"/>
-      <c r="G4" s="284"/>
+      <c r="B4" s="271"/>
+      <c r="C4" s="296"/>
+      <c r="D4" s="297"/>
+      <c r="E4" s="290"/>
+      <c r="F4" s="291"/>
+      <c r="G4" s="292"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="317"/>
-      <c r="C5" s="288"/>
-      <c r="D5" s="289"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="287"/>
+      <c r="B5" s="271"/>
+      <c r="C5" s="296"/>
+      <c r="D5" s="297"/>
+      <c r="E5" s="293"/>
+      <c r="F5" s="294"/>
+      <c r="G5" s="295"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="317"/>
-      <c r="C6" s="288"/>
-      <c r="D6" s="289"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="286"/>
-      <c r="G6" s="287"/>
+      <c r="B6" s="271"/>
+      <c r="C6" s="296"/>
+      <c r="D6" s="297"/>
+      <c r="E6" s="293"/>
+      <c r="F6" s="294"/>
+      <c r="G6" s="295"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="317"/>
-      <c r="C7" s="288"/>
-      <c r="D7" s="289"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="286"/>
-      <c r="G7" s="287"/>
+      <c r="B7" s="271"/>
+      <c r="C7" s="296"/>
+      <c r="D7" s="297"/>
+      <c r="E7" s="293"/>
+      <c r="F7" s="294"/>
+      <c r="G7" s="295"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="317"/>
+      <c r="B8" s="271"/>
       <c r="C8" s="260"/>
       <c r="D8" s="261"/>
       <c r="E8" s="257"/>
@@ -9335,7 +9600,7 @@
       <c r="G8" s="259"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="317"/>
+      <c r="B9" s="271"/>
       <c r="C9" s="260"/>
       <c r="D9" s="261"/>
       <c r="E9" s="257"/>
@@ -9343,7 +9608,7 @@
       <c r="G9" s="259"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="317"/>
+      <c r="B10" s="271"/>
       <c r="C10" s="260"/>
       <c r="D10" s="261"/>
       <c r="E10" s="257"/>
@@ -9351,7 +9616,7 @@
       <c r="G10" s="259"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="317"/>
+      <c r="B11" s="271"/>
       <c r="C11" s="260"/>
       <c r="D11" s="261"/>
       <c r="E11" s="257"/>
@@ -9359,7 +9624,7 @@
       <c r="G11" s="259"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="317"/>
+      <c r="B12" s="271"/>
       <c r="C12" s="260"/>
       <c r="D12" s="261"/>
       <c r="E12" s="257"/>
@@ -9367,7 +9632,7 @@
       <c r="G12" s="259"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="317"/>
+      <c r="B13" s="271"/>
       <c r="C13" s="260"/>
       <c r="D13" s="261"/>
       <c r="E13" s="257"/>
@@ -9375,7 +9640,7 @@
       <c r="G13" s="259"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="317"/>
+      <c r="B14" s="271"/>
       <c r="C14" s="260"/>
       <c r="D14" s="261"/>
       <c r="E14" s="257"/>
@@ -9383,7 +9648,7 @@
       <c r="G14" s="259"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="317"/>
+      <c r="B15" s="271"/>
       <c r="C15" s="260"/>
       <c r="D15" s="261"/>
       <c r="E15" s="257"/>
@@ -9391,7 +9656,7 @@
       <c r="G15" s="259"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="317"/>
+      <c r="B16" s="271"/>
       <c r="C16" s="260"/>
       <c r="D16" s="261"/>
       <c r="E16" s="257"/>
@@ -9399,7 +9664,7 @@
       <c r="G16" s="259"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="317"/>
+      <c r="B17" s="271"/>
       <c r="C17" s="260"/>
       <c r="D17" s="261"/>
       <c r="E17" s="257"/>
@@ -9407,7 +9672,7 @@
       <c r="G17" s="259"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="317"/>
+      <c r="B18" s="271"/>
       <c r="C18" s="260"/>
       <c r="D18" s="261"/>
       <c r="E18" s="257"/>
@@ -9415,7 +9680,7 @@
       <c r="G18" s="259"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="317"/>
+      <c r="B19" s="271"/>
       <c r="C19" s="260"/>
       <c r="D19" s="261"/>
       <c r="E19" s="257"/>
@@ -9423,7 +9688,7 @@
       <c r="G19" s="259"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="317"/>
+      <c r="B20" s="271"/>
       <c r="C20" s="260"/>
       <c r="D20" s="261"/>
       <c r="E20" s="257"/>
@@ -9431,7 +9696,7 @@
       <c r="G20" s="259"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="317"/>
+      <c r="B21" s="271"/>
       <c r="C21" s="260"/>
       <c r="D21" s="261"/>
       <c r="E21" s="257"/>
@@ -9439,7 +9704,7 @@
       <c r="G21" s="259"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="317"/>
+      <c r="B22" s="271"/>
       <c r="C22" s="260"/>
       <c r="D22" s="261"/>
       <c r="E22" s="257"/>
@@ -9447,7 +9712,7 @@
       <c r="G22" s="259"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="317"/>
+      <c r="B23" s="271"/>
       <c r="C23" s="260"/>
       <c r="D23" s="261"/>
       <c r="E23" s="257"/>
@@ -9455,7 +9720,7 @@
       <c r="G23" s="259"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="317"/>
+      <c r="B24" s="271"/>
       <c r="C24" s="260"/>
       <c r="D24" s="261"/>
       <c r="E24" s="257"/>
@@ -9463,7 +9728,7 @@
       <c r="G24" s="259"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="317"/>
+      <c r="B25" s="271"/>
       <c r="C25" s="260"/>
       <c r="D25" s="261"/>
       <c r="E25" s="257"/>
@@ -9471,7 +9736,7 @@
       <c r="G25" s="259"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="317"/>
+      <c r="B26" s="271"/>
       <c r="C26" s="260"/>
       <c r="D26" s="261"/>
       <c r="E26" s="257"/>
@@ -9479,7 +9744,7 @@
       <c r="G26" s="259"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="317"/>
+      <c r="B27" s="271"/>
       <c r="C27" s="260"/>
       <c r="D27" s="261"/>
       <c r="E27" s="257"/>
@@ -9487,7 +9752,7 @@
       <c r="G27" s="259"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="317"/>
+      <c r="B28" s="271"/>
       <c r="C28" s="260"/>
       <c r="D28" s="261"/>
       <c r="E28" s="257"/>
@@ -9495,71 +9760,89 @@
       <c r="G28" s="259"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="317"/>
-      <c r="C29" s="288"/>
-      <c r="D29" s="289"/>
-      <c r="E29" s="285"/>
-      <c r="F29" s="286"/>
-      <c r="G29" s="287"/>
+      <c r="B29" s="271"/>
+      <c r="C29" s="296"/>
+      <c r="D29" s="297"/>
+      <c r="E29" s="293"/>
+      <c r="F29" s="294"/>
+      <c r="G29" s="295"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="317"/>
-      <c r="C30" s="288"/>
-      <c r="D30" s="289"/>
-      <c r="E30" s="285"/>
-      <c r="F30" s="286"/>
-      <c r="G30" s="287"/>
+      <c r="B30" s="271"/>
+      <c r="C30" s="296"/>
+      <c r="D30" s="297"/>
+      <c r="E30" s="293"/>
+      <c r="F30" s="294"/>
+      <c r="G30" s="295"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="317"/>
-      <c r="C31" s="288"/>
-      <c r="D31" s="289"/>
-      <c r="E31" s="285"/>
-      <c r="F31" s="286"/>
-      <c r="G31" s="287"/>
+      <c r="B31" s="271"/>
+      <c r="C31" s="296"/>
+      <c r="D31" s="297"/>
+      <c r="E31" s="293"/>
+      <c r="F31" s="294"/>
+      <c r="G31" s="295"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="317"/>
-      <c r="C32" s="288"/>
-      <c r="D32" s="289"/>
-      <c r="E32" s="285"/>
-      <c r="F32" s="286"/>
-      <c r="G32" s="287"/>
+      <c r="B32" s="271"/>
+      <c r="C32" s="296"/>
+      <c r="D32" s="297"/>
+      <c r="E32" s="293"/>
+      <c r="F32" s="294"/>
+      <c r="G32" s="295"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="317"/>
-      <c r="C33" s="288"/>
-      <c r="D33" s="289"/>
-      <c r="E33" s="285"/>
-      <c r="F33" s="286"/>
-      <c r="G33" s="287"/>
+      <c r="B33" s="271"/>
+      <c r="C33" s="296"/>
+      <c r="D33" s="297"/>
+      <c r="E33" s="293"/>
+      <c r="F33" s="294"/>
+      <c r="G33" s="295"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="317"/>
-      <c r="C34" s="288"/>
-      <c r="D34" s="289"/>
-      <c r="E34" s="285"/>
-      <c r="F34" s="286"/>
-      <c r="G34" s="287"/>
+      <c r="B34" s="271"/>
+      <c r="C34" s="296"/>
+      <c r="D34" s="297"/>
+      <c r="E34" s="293"/>
+      <c r="F34" s="294"/>
+      <c r="G34" s="295"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="317"/>
-      <c r="C35" s="288"/>
-      <c r="D35" s="289"/>
-      <c r="E35" s="285"/>
-      <c r="F35" s="286"/>
-      <c r="G35" s="287"/>
+      <c r="B35" s="271"/>
+      <c r="C35" s="296"/>
+      <c r="D35" s="297"/>
+      <c r="E35" s="293"/>
+      <c r="F35" s="294"/>
+      <c r="G35" s="295"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="317"/>
-      <c r="C36" s="288"/>
-      <c r="D36" s="289"/>
-      <c r="E36" s="285"/>
-      <c r="F36" s="286"/>
-      <c r="G36" s="287"/>
+      <c r="B36" s="271"/>
+      <c r="C36" s="296"/>
+      <c r="D36" s="297"/>
+      <c r="E36" s="293"/>
+      <c r="F36" s="294"/>
+      <c r="G36" s="295"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="C36:D36"/>
@@ -9570,24 +9853,6 @@
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:G34"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>